<commit_message>
added some basic functions to save status of checked domains inside a new excel file
</commit_message>
<xml_diff>
--- a/exampleExcel.xlsx
+++ b/exampleExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\OneDrive\Dokumenter\VSCode\Java projects\Webcrawlers\webcrawler_dyson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A14404-74A1-4665-BA72-1A4DFA9FF0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DE26ED-09D4-4D11-B7C1-80676BFF7E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23940" yWindow="1395" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -411,7 +411,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,9 +460,7 @@
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3">
-        <v>200</v>
-      </c>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -471,9 +469,7 @@
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3">
-        <v>200</v>
-      </c>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -482,9 +478,7 @@
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3">
-        <v>200</v>
-      </c>
+      <c r="C6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>